<commit_message>
Improved parsing, storage in folder, naming convention
</commit_message>
<xml_diff>
--- a/proba.xlsx
+++ b/proba.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="41260" yWindow="4920" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="51200" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,35 +29,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test 2</t>
-  </si>
-  <si>
-    <t>test 3</t>
-  </si>
-  <si>
-    <t>test 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proba1 </t>
-  </si>
-  <si>
-    <t>proba 2</t>
-  </si>
-  <si>
-    <t>proba 3</t>
+    <t>Kolona 1</t>
+  </si>
+  <si>
+    <t>Kolona 2</t>
+  </si>
+  <si>
+    <t>Kolona 3</t>
+  </si>
+  <si>
+    <t>Kolona 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vrijednost </t>
+  </si>
+  <si>
+    <t>nerminsehic1993@gmail.com</t>
+  </si>
+  <si>
+    <t>bla bla 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,13 +88,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -363,13 +373,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -385,33 +398,24 @@
         <v>3</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>